<commit_message>
added some code in UI suite
</commit_message>
<xml_diff>
--- a/Data/RegressionUI.xlsx
+++ b/Data/RegressionUI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshverma/IdeaProjects/AutomationPack/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE44E3B8-3EA3-8C4A-9F4A-BFD7039B5CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9935646F-ADB4-3B4A-8DCA-5DE8B1EE45E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17040" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>Run</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98AFFF1-155B-3D48-B506-BB77B198CD56}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,7 +443,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>4</v>
@@ -462,9 +465,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="s" s="0">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added code for timesheet update
</commit_message>
<xml_diff>
--- a/Data/RegressionUI.xlsx
+++ b/Data/RegressionUI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshverma/IdeaProjects/AutomationPack/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9935646F-ADB4-3B4A-8DCA-5DE8B1EE45E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C1BDC6-9CA8-1A4C-A823-84DACC4B4267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17040" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
+    <workbookView xWindow="1360" yWindow="780" windowWidth="28040" windowHeight="17040" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
   </bookViews>
   <sheets>
     <sheet name="timeSheet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Run</t>
   </si>
@@ -49,10 +49,19 @@
     <t>yes</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
     <t>done</t>
   </si>
   <si>
-    <t>no</t>
+    <t xml:space="preserve">ACME Ltd </t>
   </si>
 </sst>
 </file>
@@ -60,10 +69,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,18 +420,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98AFFF1-155B-3D48-B506-BB77B198CD56}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.57421875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="38.5"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.57421875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
@@ -424,10 +440,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -435,48 +457,47 @@
         <v>3</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="s" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added code for attendance
</commit_message>
<xml_diff>
--- a/Data/RegressionUI.xlsx
+++ b/Data/RegressionUI.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshverma/IdeaProjects/AutomationPack/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57484F44-0666-5349-9E1F-9ECF83012117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472F6D94-BFA2-824F-BBA2-000EA9E13043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17040" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
   </bookViews>
   <sheets>
     <sheet name="timeSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="attendance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Run</t>
   </si>
@@ -68,13 +69,27 @@
   </si>
   <si>
     <t>hours</t>
+  </si>
+  <si>
+    <t>Punch In Time</t>
+  </si>
+  <si>
+    <t>Punch Out Time</t>
+  </si>
+  <si>
+    <t>09:00 AM</t>
+  </si>
+  <si>
+    <t>06:00 PM</t>
+  </si>
+  <si>
+    <t>9:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,93 +446,176 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98AFFF1-155B-3D48-B506-BB77B198CD56}">
   <dimension ref="A1:F5"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C547F82-3024-0A4B-8E33-0958B8DFFD0A}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="38.5"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125"/>
-    <col min="5" max="5" customWidth="true" width="14.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.57421875"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s" s="0">
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>8</v>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>8</v>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>8</v>
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added PIM edit code
</commit_message>
<xml_diff>
--- a/Data/RegressionUI.xlsx
+++ b/Data/RegressionUI.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshverma/IdeaProjects/AutomationPack/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ECB2C0-6C1B-3948-89F9-723D4FABCF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9722012-14E6-F345-882A-119B023BD86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16920" activeTab="2" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
   </bookViews>
   <sheets>
     <sheet name="timeSheet" sheetId="1" r:id="rId1"/>
     <sheet name="attendance" sheetId="2" r:id="rId2"/>
+    <sheet name="pimUpdate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>Run</t>
   </si>
@@ -84,6 +85,12 @@
   </si>
   <si>
     <t>9:00</t>
+  </si>
+  <si>
+    <t>Blood Group</t>
+  </si>
+  <si>
+    <t>O+</t>
   </si>
 </sst>
 </file>
@@ -448,7 +455,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="C5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C547F82-3024-0A4B-8E33-0958B8DFFD0A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -620,4 +627,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275B3916-9281-9B4E-9587-223060CB0ABA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.57421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added stream instead of for loop, while handling web elements
</commit_message>
<xml_diff>
--- a/Data/RegressionUI.xlsx
+++ b/Data/RegressionUI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshverma/IdeaProjects/AutomationPack/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9722012-14E6-F345-882A-119B023BD86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E52C7F-6780-1A49-A7D9-7AF1112DDF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16920" activeTab="2" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="28040" windowHeight="16620" activeTab="2" xr2:uid="{6B8C0FC8-8986-4A42-A027-2171E9EAAECE}"/>
   </bookViews>
   <sheets>
     <sheet name="timeSheet" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>Run</t>
   </si>
@@ -90,7 +90,19 @@
     <t>Blood Group</t>
   </si>
   <si>
-    <t>O+</t>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>ninja</t>
   </si>
 </sst>
 </file>
@@ -463,7 +475,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="38.5"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.33203125"/>
     <col min="5" max="5" customWidth="true" width="14.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.57421875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -631,18 +643,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275B3916-9281-9B4E-9587-223060CB0ABA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.57421875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.1640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.57421875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
@@ -650,27 +663,39 @@
         <v>0</v>
       </c>
       <c r="C1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="E1" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="0">
         <v>2</v>
       </c>
@@ -678,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="0">
         <v>3</v>
       </c>
@@ -686,7 +711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="0">
         <v>4</v>
       </c>

</xml_diff>